<commit_message>
Update data and pdf
</commit_message>
<xml_diff>
--- a/data/TBC_Tracker_scrapped.xlsx
+++ b/data/TBC_Tracker_scrapped.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="55">
   <si>
     <t>Date</t>
   </si>
@@ -120,7 +120,7 @@
     <t>Elus</t>
   </si>
   <si>
-    <t>Clarisse</t>
+    <t>Odette</t>
   </si>
   <si>
     <t>Fouquet’s</t>
@@ -151,6 +151,33 @@
   </si>
   <si>
     <t>Ma meilleure :"Vous parlez pas de fusion nucléaire dans la partie énergie!?"</t>
+  </si>
+  <si>
+    <t>Université ou grande école</t>
+  </si>
+  <si>
+    <t>ENSEEIHT</t>
+  </si>
+  <si>
+    <t>Peu de monde, beaucoup de connaisseurs</t>
+  </si>
+  <si>
+    <t>Peu de monde, moins de connaisseurs que la veille</t>
+  </si>
+  <si>
+    <t>Corentin Douellou</t>
+  </si>
+  <si>
+    <t>Clermont-Ferrand</t>
+  </si>
+  <si>
+    <t>Laboratoire UMR</t>
+  </si>
+  <si>
+    <t>Institut Pascal</t>
+  </si>
+  <si>
+    <t>Intéréssés et retours positifs sur le fond et la forme de la conf. Mais pas tous convaincus à arrêter de prendre l'avion pour aller en conf aux USA ou en Thailande.</t>
   </si>
 </sst>
 </file>
@@ -193,7 +220,6 @@
       <name val="Arial"/>
     </font>
     <font>
-      <color theme="1"/>
       <name val="Roboto"/>
     </font>
   </fonts>
@@ -225,7 +251,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -245,6 +271,9 @@
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -271,6 +300,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -540,16 +572,16 @@
       <c r="E2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="9">
         <v>20.0</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="10">
         <v>3.0</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>15</v>
       </c>
     </row>
@@ -569,16 +601,16 @@
       <c r="E3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="9">
         <v>35.0</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="10">
         <v>3.0</v>
       </c>
-      <c r="I3" s="11"/>
+      <c r="I3" s="12"/>
     </row>
     <row r="4">
       <c r="A4" s="5">
@@ -596,16 +628,16 @@
       <c r="E4" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="9">
         <v>60.0</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="10">
         <v>3.0</v>
       </c>
-      <c r="I4" s="11"/>
+      <c r="I4" s="12"/>
     </row>
     <row r="5">
       <c r="A5" s="5">
@@ -623,16 +655,16 @@
       <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="9">
         <v>20.0</v>
       </c>
-      <c r="H5" s="9">
+      <c r="H5" s="10">
         <v>3.0</v>
       </c>
-      <c r="I5" s="11"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6">
       <c r="A6" s="5">
@@ -650,16 +682,16 @@
       <c r="E6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="9">
         <v>50.0</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="10">
         <v>2.0</v>
       </c>
-      <c r="I6" s="11"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7">
       <c r="A7" s="5">
@@ -677,23 +709,23 @@
       <c r="E7" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="9">
         <v>30.0</v>
       </c>
-      <c r="H7" s="9">
+      <c r="H7" s="10">
         <v>2.0</v>
       </c>
-      <c r="I7" s="11"/>
-      <c r="L7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="L7" s="13"/>
     </row>
     <row r="8">
       <c r="A8" s="5">
         <v>43217.0</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -705,16 +737,16 @@
       <c r="E8" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="9">
         <v>40.0</v>
       </c>
-      <c r="H8" s="9">
+      <c r="H8" s="10">
         <v>2.0</v>
       </c>
-      <c r="I8" s="11"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9">
       <c r="A9" s="5">
@@ -729,17 +761,17 @@
       <c r="D9" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="15"/>
+      <c r="F9" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="9">
         <v>55.0</v>
       </c>
-      <c r="H9" s="9">
+      <c r="H9" s="10">
         <v>2.0</v>
       </c>
-      <c r="I9" s="11"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10">
       <c r="A10" s="5">
@@ -754,247 +786,301 @@
       <c r="D10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="14"/>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="15"/>
+      <c r="F10" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="9">
         <v>25.0</v>
       </c>
-      <c r="H10" s="9">
+      <c r="H10" s="10">
         <v>1.0</v>
       </c>
-      <c r="I10" s="11"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11">
-      <c r="A11" s="15">
+      <c r="A11" s="16">
         <v>43668.0</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="11" t="s">
         <v>42</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G11" s="10">
+      <c r="G11" s="11">
         <v>50.0</v>
       </c>
-      <c r="H11" s="9">
+      <c r="H11" s="10">
         <v>2.0</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="17" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="15"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="11"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="A12" s="18">
+        <v>43719.0</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="10">
+        <v>14.0</v>
+      </c>
+      <c r="H12" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="15"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="11"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="A13" s="18">
+        <v>43720.0</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="10">
+        <v>12.0</v>
+      </c>
+      <c r="H13" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="I13" s="10" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="15"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
+      <c r="A14" s="18">
+        <v>43563.0</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" s="10">
+        <v>20.0</v>
+      </c>
+      <c r="H14" s="10">
+        <v>3.0</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="15"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="11"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="11"/>
+      <c r="C15" s="12"/>
       <c r="D15" s="7"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
+      <c r="E15" s="12"/>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="12"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16">
-      <c r="A16" s="15"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="11"/>
+      <c r="A16" s="16"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="12"/>
       <c r="D16" s="7"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="11"/>
-      <c r="G16" s="11"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="11"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="12"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17">
-      <c r="A17" s="15"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="11"/>
+      <c r="A17" s="16"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="12"/>
       <c r="D17" s="7"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="11"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="12"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18">
-      <c r="A18" s="15"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+      <c r="A18" s="16"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
       <c r="D18" s="7"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19">
-      <c r="A19" s="15"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+      <c r="A19" s="16"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
       <c r="D19" s="7"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20">
-      <c r="A20" s="15"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+      <c r="A20" s="16"/>
+      <c r="B20" s="12"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="7"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="12"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21">
-      <c r="A21" s="15"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="A21" s="16"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="7"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22">
-      <c r="A22" s="15"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
+      <c r="A22" s="16"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="12"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23">
-      <c r="A23" s="15"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
+      <c r="A23" s="16"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="7"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+      <c r="G23" s="12"/>
+      <c r="H23" s="12"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24">
-      <c r="A24" s="15"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="A24" s="16"/>
+      <c r="B24" s="12"/>
+      <c r="C24" s="12"/>
       <c r="D24" s="7"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="12"/>
+      <c r="H24" s="12"/>
+      <c r="I24" s="12"/>
     </row>
     <row r="25">
-      <c r="A25" s="15"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
+      <c r="A25" s="16"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="7"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26">
-      <c r="A26" s="15"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+      <c r="A26" s="16"/>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
       <c r="D26" s="7"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="11"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27">
-      <c r="A27" s="15"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="A27" s="16"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="12"/>
       <c r="D27" s="7"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="12"/>
+      <c r="H27" s="12"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28">
-      <c r="A28" s="15"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="A28" s="16"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="7"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29">
-      <c r="A29" s="15"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
+      <c r="A29" s="16"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="12"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="12"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="$B$1:$I$29"/>
@@ -1002,12 +1088,6 @@
     <dataValidation type="list" allowBlank="1" sqref="F2:F29">
       <formula1>"Étudiants,Travail,Proches,Public,Elus,Journalistes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D2 D4:D29">
-      <formula1>"Université ou grande école,Collège,Lycée,Ecole primaire,Bar,Salle de village,Travail,Parti politique"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="D3">
-      <formula1>"Université ou grande école,Collège,Lycée,Ecole primaire,Bar,Salle de village,Travail,Parti politique,Maison associative"</formula1>
-    </dataValidation>
   </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Add ceiling of legend breaks
</commit_message>
<xml_diff>
--- a/data/TBC_Tracker_scrapped.xlsx
+++ b/data/TBC_Tracker_scrapped.xlsx
@@ -7,14 +7,14 @@
     <sheet state="visible" name="CONSIGNES REMPLISSAGE" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$B$1:$J$32</definedName>
+    <definedName hidden="1" localSheetId="0" name="_xlnm._FilterDatabase">'Feuille 1'!$B$1:$J$40</definedName>
   </definedNames>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="165">
   <si>
     <t>CONSIGNES REMPLISSAGE FEUILLE</t>
   </si>
@@ -429,6 +429,87 @@
   </si>
   <si>
     <t>Public intéressé, quelques uns connaissaient la question, mais pas la majorité</t>
+  </si>
+  <si>
+    <t>Antony</t>
+  </si>
+  <si>
+    <t>Salle municipale</t>
+  </si>
+  <si>
+    <t>Salle Henri Lasson</t>
+  </si>
+  <si>
+    <t>Public intéressé, hétérogène en terme de connaissance sur le sujet, long débat sur e nucléaire pendant les questions</t>
+  </si>
+  <si>
+    <t>Nanterre</t>
+  </si>
+  <si>
+    <t>Université de Nanterre</t>
+  </si>
+  <si>
+    <t>Conf en version ultra-courte (20 min), public connaisseur, intéressé mais peu de questions</t>
+  </si>
+  <si>
+    <t>Marie-Laure &amp; Léopoldine</t>
+  </si>
+  <si>
+    <t>Théâtre</t>
+  </si>
+  <si>
+    <t>L'improvibar</t>
+  </si>
+  <si>
+    <t>Public peu informé, intéressés, envie de creuser</t>
+  </si>
+  <si>
+    <t>LieU'topie</t>
+  </si>
+  <si>
+    <t>Public assez connaisseur</t>
+  </si>
+  <si>
+    <t>Bergerac</t>
+  </si>
+  <si>
+    <t>Centre social</t>
+  </si>
+  <si>
+    <t>Centre social Germaine Tillon</t>
+  </si>
+  <si>
+    <t>Conf Blac Bordeaux, invité par Colibris Bergerac, avec atelier sur les imaginaires</t>
+  </si>
+  <si>
+    <t>Pourquoi y'a pas le solaire thermique et la micro-hydro sur votre graphique en 2 axes ?</t>
+  </si>
+  <si>
+    <t>Hanitra</t>
+  </si>
+  <si>
+    <t>Castillon</t>
+  </si>
+  <si>
+    <t>Invité par Castillonnais en transition</t>
+  </si>
+  <si>
+    <t>Lise, Vadim</t>
+  </si>
+  <si>
+    <t>A2 Consulting</t>
+  </si>
+  <si>
+    <t>Bien, mais plutôt des personnes déjà renseignées étaient présentes</t>
+  </si>
+  <si>
+    <t>Lise, Vincent Iva</t>
+  </si>
+  <si>
+    <t>Station E</t>
+  </si>
+  <si>
+    <t>Mini format Quizz avec quelques graph imprimés, pas de video proj + atelier en sous-groupe sur actions pour chaque secteur consommateur d'énergie</t>
   </si>
 </sst>
 </file>
@@ -440,7 +521,7 @@
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -458,10 +539,6 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Cambria"/>
     </font>
     <font>
       <sz val="14.0"/>
@@ -498,7 +575,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -514,10 +591,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="3" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -526,14 +606,14 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -542,14 +622,17 @@
     <xf borderId="1" fillId="0" fontId="1" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -767,7 +850,10 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
@@ -822,27 +908,27 @@
       <c r="D2" s="7">
         <v>38.0</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H2" s="5">
         <v>20.0</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="9">
         <v>2.0</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="9">
+      <c r="A3" s="10">
         <v>43517.0</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -854,25 +940,25 @@
       <c r="D3" s="7">
         <v>31.0</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="8" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H3" s="5">
         <v>60.0</v>
       </c>
-      <c r="I3" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J3" s="10"/>
+      <c r="I3" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J3" s="11"/>
     </row>
     <row r="4" hidden="1">
-      <c r="A4" s="9">
+      <c r="A4" s="10">
         <v>43631.0</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -884,52 +970,52 @@
       <c r="D4" s="7">
         <v>66.0</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="8" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="5">
         <v>20.0</v>
       </c>
-      <c r="I4" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J4" s="10"/>
+      <c r="I4" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J4" s="11"/>
     </row>
     <row r="5">
-      <c r="A5" s="11">
+      <c r="A5" s="12">
         <v>43668.0</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="7">
         <v>78.0</v>
       </c>
-      <c r="E5" s="7" t="s">
+      <c r="E5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="8" t="s">
+      <c r="F5" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="G5" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="8">
+      <c r="H5" s="9">
         <v>50.0</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="9">
         <v>2.0</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="J5" s="9" t="s">
         <v>31</v>
       </c>
       <c r="K5" s="1" t="s">
@@ -937,378 +1023,380 @@
       </c>
     </row>
     <row r="6" hidden="1">
-      <c r="A6" s="11">
+      <c r="A6" s="12">
         <v>43719.0</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="7">
         <v>31.0</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="8">
+      <c r="H6" s="9">
         <v>14.0</v>
       </c>
-      <c r="I6" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J6" s="8" t="s">
+      <c r="I6" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J6" s="9" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="11">
+      <c r="A7" s="12">
         <v>43720.0</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="9" t="s">
         <v>21</v>
       </c>
       <c r="D7" s="7">
         <v>31.0</v>
       </c>
-      <c r="E7" s="7" t="s">
+      <c r="E7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="9">
         <v>12.0</v>
       </c>
-      <c r="I7" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J7" s="9" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="11">
+      <c r="A8" s="12">
         <v>43563.0</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="9" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="7">
         <v>63.0</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="8" t="s">
+      <c r="F8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H8" s="8">
+      <c r="H8" s="9">
         <v>20.0</v>
       </c>
-      <c r="I8" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J8" s="8" t="s">
+      <c r="I8" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="11">
+      <c r="A9" s="12">
         <v>43560.0</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D9" s="7">
         <v>60.0</v>
       </c>
-      <c r="E9" s="7" t="s">
+      <c r="E9" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F9" s="8" t="s">
+      <c r="F9" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H9" s="8">
+      <c r="H9" s="9">
         <v>30.0</v>
       </c>
-      <c r="I9" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J9" s="8" t="s">
+      <c r="I9" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="11">
+      <c r="A10" s="12">
         <v>43624.0</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="9" t="s">
         <v>43</v>
       </c>
       <c r="D10" s="7">
         <v>60.0</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="8" t="s">
+      <c r="F10" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="8">
+      <c r="H10" s="9">
         <v>20.0</v>
       </c>
-      <c r="I10" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J10" s="8" t="s">
+      <c r="I10" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J10" s="9" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="11">
+      <c r="A11" s="12">
         <v>43539.0</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="9" t="s">
         <v>51</v>
       </c>
       <c r="D11" s="7">
         <v>14.0</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="F11" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="8">
+      <c r="H11" s="9">
         <v>70.0</v>
       </c>
-      <c r="I11" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J11" s="8" t="s">
+      <c r="I11" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="11">
+      <c r="A12" s="12">
         <v>43532.0</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C12" s="9" t="s">
         <v>56</v>
       </c>
       <c r="D12" s="7">
         <v>93.0</v>
       </c>
-      <c r="E12" s="7" t="s">
+      <c r="E12" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="8">
+      <c r="H12" s="9">
         <v>30.0</v>
       </c>
-      <c r="I12" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J12" s="10"/>
+      <c r="I12" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J12" s="11"/>
     </row>
     <row r="13">
-      <c r="A13" s="11">
+      <c r="A13" s="12">
         <v>43608.0</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="9" t="s">
         <v>59</v>
       </c>
       <c r="D13" s="7">
         <v>75.0</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="E13" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="9">
         <v>60.0</v>
       </c>
-      <c r="I13" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J13" s="10"/>
+      <c r="I13" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J13" s="11"/>
     </row>
     <row r="14">
-      <c r="A14" s="11">
+      <c r="A14" s="12">
         <v>43531.0</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="9" t="s">
         <v>61</v>
       </c>
       <c r="D14" s="7">
         <v>94.0</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="E14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="8" t="s">
+      <c r="F14" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="G14" s="8" t="s">
+      <c r="G14" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H14" s="9">
         <v>15.0</v>
       </c>
-      <c r="I14" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J14" s="10"/>
+      <c r="I14" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J14" s="11"/>
     </row>
     <row r="15">
-      <c r="A15" s="11">
+      <c r="A15" s="12">
         <v>43622.0</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="9" t="s">
         <v>59</v>
       </c>
       <c r="D15" s="7">
         <v>75.0</v>
       </c>
-      <c r="E15" s="7" t="s">
+      <c r="E15" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F15" s="8" t="s">
+      <c r="F15" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="8" t="s">
+      <c r="G15" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H15" s="8">
+      <c r="H15" s="9">
         <v>10.0</v>
       </c>
-      <c r="I15" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J15" s="8" t="s">
+      <c r="I15" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J15" s="9" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="11">
+      <c r="A16" s="12">
         <v>43623.0</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9" t="s">
         <v>59</v>
       </c>
       <c r="D16" s="7">
         <v>75.0</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="F16" s="8" t="s">
+      <c r="F16" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="G16" s="8" t="s">
+      <c r="G16" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="9">
         <v>10.0</v>
       </c>
-      <c r="I16" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J16" s="8" t="s">
+      <c r="I16" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J16" s="9" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="11">
+      <c r="A17" s="12">
         <v>43164.0</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7" t="s">
+      <c r="D17" s="7">
+        <v>26.0</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="G17" s="8" t="s">
+      <c r="G17" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="8">
+      <c r="H17" s="9">
         <v>30.0</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="9">
         <v>2.0</v>
       </c>
-      <c r="J17" s="8" t="s">
+      <c r="J17" s="9" t="s">
         <v>73</v>
       </c>
       <c r="K17" s="1" t="s">
@@ -1316,374 +1404,374 @@
       </c>
     </row>
     <row r="18" hidden="1">
-      <c r="A18" s="11">
+      <c r="A18" s="12">
         <v>43260.0</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="9" t="s">
         <v>75</v>
       </c>
       <c r="D18" s="7"/>
-      <c r="E18" s="7" t="s">
+      <c r="E18" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="F18" s="8" t="s">
+      <c r="F18" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="G18" s="8" t="s">
+      <c r="G18" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H18" s="8">
+      <c r="H18" s="9">
         <v>5.0</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="9">
         <v>2.0</v>
       </c>
-      <c r="J18" s="8" t="s">
+      <c r="J18" s="9" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="11">
+      <c r="A19" s="12">
         <v>43439.0</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C19" s="8" t="s">
+      <c r="C19" s="9" t="s">
         <v>80</v>
       </c>
       <c r="D19" s="7">
         <v>94.0</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="8" t="s">
+      <c r="F19" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="8" t="s">
+      <c r="G19" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="9">
         <v>16.0</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="9">
         <v>2.0</v>
       </c>
-      <c r="J19" s="8" t="s">
+      <c r="J19" s="9" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="11">
+      <c r="A20" s="12">
         <v>43146.0</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="9" t="s">
         <v>85</v>
       </c>
       <c r="D20" s="7">
         <v>78.0</v>
       </c>
-      <c r="E20" s="7" t="s">
+      <c r="E20" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="8" t="s">
+      <c r="F20" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="G20" s="8" t="s">
+      <c r="G20" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="9">
         <v>25.0</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="9">
         <v>2.0</v>
       </c>
-      <c r="J20" s="10"/>
+      <c r="J20" s="11"/>
     </row>
     <row r="21" hidden="1">
-      <c r="A21" s="11">
+      <c r="A21" s="12">
         <v>43741.0</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="9" t="s">
         <v>87</v>
       </c>
       <c r="D21" s="7">
         <v>69.0</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="E21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="F21" s="8" t="s">
+      <c r="F21" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="G21" s="8" t="s">
+      <c r="G21" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H21" s="8">
+      <c r="H21" s="9">
         <v>45.0</v>
       </c>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="11"/>
     </row>
     <row r="22" hidden="1">
-      <c r="A22" s="11">
+      <c r="A22" s="12">
         <v>43539.0</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="9" t="s">
         <v>90</v>
       </c>
       <c r="D22" s="7">
         <v>57.0</v>
       </c>
-      <c r="E22" s="7" t="s">
+      <c r="E22" s="8" t="s">
         <v>91</v>
       </c>
-      <c r="F22" s="8" t="s">
+      <c r="F22" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H22" s="12">
+      <c r="H22" s="13">
         <v>11.0</v>
       </c>
-      <c r="I22" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J22" s="8" t="s">
+      <c r="I22" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J22" s="9" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="11">
+      <c r="A23" s="12">
         <v>43605.0</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="9" t="s">
         <v>90</v>
       </c>
       <c r="D23" s="7">
         <v>57.0</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="E23" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="8" t="s">
+      <c r="F23" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G23" s="8" t="s">
+      <c r="G23" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H23" s="8">
+      <c r="H23" s="9">
         <v>40.0</v>
       </c>
-      <c r="I23" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J23" s="8" t="s">
+      <c r="I23" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J23" s="9" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="13">
+      <c r="A24" s="14">
         <v>43634.0</v>
       </c>
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="C24" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="10"/>
-      <c r="E24" s="8" t="s">
+      <c r="D24" s="11"/>
+      <c r="E24" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="10"/>
-      <c r="G24" s="8" t="s">
+      <c r="F24" s="11"/>
+      <c r="G24" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H24" s="8">
+      <c r="H24" s="9">
         <v>15.0</v>
       </c>
-      <c r="I24" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J24" s="8" t="s">
+      <c r="I24" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J24" s="9" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="14">
+      <c r="A25" s="15">
         <v>43398.0</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="9">
         <v>24.0</v>
       </c>
-      <c r="E25" s="8" t="s">
+      <c r="E25" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="F25" s="8" t="s">
+      <c r="F25" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="G25" s="8" t="s">
+      <c r="G25" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H25" s="8">
+      <c r="H25" s="9">
         <v>50.0</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="9">
         <v>1.0</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="9" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="13">
+      <c r="A26" s="14">
         <v>43213.0</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="C26" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="9">
         <v>33.0</v>
       </c>
-      <c r="E26" s="8" t="s">
+      <c r="E26" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="F26" s="8" t="s">
+      <c r="F26" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="G26" s="8" t="s">
+      <c r="G26" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="8">
+      <c r="H26" s="9">
         <v>15.0</v>
       </c>
-      <c r="I26" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J26" s="8" t="s">
+      <c r="I26" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J26" s="9" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="13">
+      <c r="A27" s="14">
         <v>43568.0</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="C27" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="9">
         <v>33.0</v>
       </c>
-      <c r="E27" s="8" t="s">
+      <c r="E27" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="F27" s="8" t="s">
+      <c r="F27" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G27" s="8" t="s">
+      <c r="G27" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H27" s="8">
+      <c r="H27" s="9">
         <v>15.0</v>
       </c>
-      <c r="I27" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J27" s="8" t="s">
+      <c r="I27" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J27" s="9" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="13">
+      <c r="A28" s="14">
         <v>43645.0</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="C28" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="9">
         <v>40.0</v>
       </c>
-      <c r="E28" s="8" t="s">
+      <c r="E28" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="F28" s="8" t="s">
+      <c r="F28" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="G28" s="8" t="s">
+      <c r="G28" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H28" s="8">
+      <c r="H28" s="9">
         <v>5.0</v>
       </c>
-      <c r="I28" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J28" s="8" t="s">
+      <c r="I28" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J28" s="9" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="13">
+      <c r="A29" s="14">
         <v>43729.0</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="C29" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="9">
         <v>33.0</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="F29" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="G29" s="8" t="s">
+      <c r="G29" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H29" s="8">
+      <c r="H29" s="9">
         <v>15.0</v>
       </c>
-      <c r="I29" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J29" s="8" t="s">
+      <c r="I29" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J29" s="9" t="s">
         <v>123</v>
       </c>
     </row>
@@ -1694,19 +1782,19 @@
       <c r="B30" s="17" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="9">
         <v>22.0</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="9" t="s">
         <v>126</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="G30" s="8" t="s">
+      <c r="G30" s="9" t="s">
         <v>18</v>
       </c>
       <c r="H30" s="1">
@@ -1717,73 +1805,340 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="14">
+      <c r="A31" s="15">
         <v>43752.0</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="C31" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="D31" s="8">
+      <c r="D31" s="9">
         <v>13.0</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="8" t="s">
+      <c r="F31" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="G31" s="8" t="s">
+      <c r="G31" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H31" s="8">
+      <c r="H31" s="9">
         <v>24.0</v>
       </c>
-      <c r="I31" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J31" s="8" t="s">
+      <c r="I31" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J31" s="9" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="14">
+      <c r="A32" s="15">
         <v>43759.0</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="9">
         <v>78.0</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="9">
         <v>30.0</v>
       </c>
-      <c r="I32" s="8">
-        <v>3.0</v>
-      </c>
-      <c r="J32" s="8" t="s">
+      <c r="I32" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J32" s="9" t="s">
         <v>137</v>
       </c>
     </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="15">
+        <v>43640.0</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C33" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D33" s="9">
+        <v>92.0</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H33" s="9">
+        <v>80.0</v>
+      </c>
+      <c r="I33" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" ht="15.75" customHeight="1">
+      <c r="A34" s="15">
+        <v>43560.0</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="D34" s="9">
+        <v>92.0</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H34" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="I34" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="14">
+        <v>43562.0</v>
+      </c>
+      <c r="B35" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="C35" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D35" s="9">
+        <v>75.0</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>147</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="9">
+        <v>40.0</v>
+      </c>
+      <c r="I35" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="15">
+        <v>43777.0</v>
+      </c>
+      <c r="B36" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="9">
+        <v>63.0</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="9">
+        <v>25.0</v>
+      </c>
+      <c r="I36" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="14">
+        <v>43778.0</v>
+      </c>
+      <c r="B37" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="D37" s="9">
+        <v>24.0</v>
+      </c>
+      <c r="E37" s="9" t="s">
+        <v>152</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>153</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H37" s="9">
+        <v>45.0</v>
+      </c>
+      <c r="I37" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="15">
+        <v>43764.0</v>
+      </c>
+      <c r="B38" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C38" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="D38" s="9">
+        <v>33.0</v>
+      </c>
+      <c r="E38" s="11"/>
+      <c r="F38" s="11"/>
+      <c r="G38" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H38" s="9">
+        <v>30.0</v>
+      </c>
+      <c r="I38" s="9">
+        <v>3.0</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="18">
+        <v>43543.0</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="D39" s="19">
+        <v>75.0</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="G39" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="19">
+        <v>20.0</v>
+      </c>
+      <c r="I39" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="J39" s="19" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="18">
+        <v>43588.0</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="19">
+        <v>93.0</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="G40" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="H40" s="19">
+        <v>8.0</v>
+      </c>
+      <c r="I40" s="19">
+        <v>3.0</v>
+      </c>
+      <c r="J40" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="11"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+      <c r="G41" s="11"/>
+      <c r="H41" s="11"/>
+      <c r="I41" s="11"/>
+      <c r="J41" s="11"/>
+    </row>
   </sheetData>
-  <autoFilter ref="$B$1:$J$32"/>
+  <autoFilter ref="$B$1:$J$40"/>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G23 G25:G32">
+    <dataValidation type="list" allowBlank="1" sqref="G2:G23 G25:G38">
       <formula1>"Étudiants,Travail,Proches,Public,Elus,Journalistes"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>